<commit_message>
Fixing RAD test Cases and Data 2.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/PaymentsELHardCoded.xlsx
+++ b/KatalonData/RADTestData/PaymentsELHardCoded.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A2CDCB-FF3F-42E4-AF57-FA48CD3C20E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{0F1F2E62-1ECD-44BD-8E8C-233C086E334B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0A483EA5-3597-437D-956E-3D53CC3EB978}"/>
+    <workbookView windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{0A483EA5-3597-437D-956E-3D53CC3EB978}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$12</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$E$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="102">
   <si>
     <t>Result</t>
   </si>
@@ -261,39 +261,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Mon Nov 08 22:38:39 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:40:05 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:41:31 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:42:56 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:44:21 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:45:49 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:47:18 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:48:43 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:50:11 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:51:39 EST 2021</t>
-  </si>
-  <si>
-    <t>Mon Nov 08 22:53:05 EST 2021</t>
-  </si>
-  <si>
     <t>BusName</t>
   </si>
   <si>
@@ -307,12 +274,82 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 19:36:00 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 19:37:24 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 19:38:05 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 19:45:37 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 19:46:14 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 19:46:51 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 19:52:41 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 19:58:31 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:35:50 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:40:56 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:42:21 EDT 2022</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:43:44 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:44:24 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:45:00 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:46:10 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:46:51 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:47:28 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:48:05 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:48:42 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:49:19 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:49:56 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 25 22:50:34 EDT 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -361,19 +398,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -390,10 +427,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -428,7 +465,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -480,7 +517,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -591,21 +628,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -622,7 +659,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -674,38 +711,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F8F8F8-AE16-4B12-9448-CA2FBF5C7D40}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F8F8F8-AE16-4B12-9448-CA2FBF5C7D40}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10" style="1" collapsed="1"/>
-    <col min="13" max="13" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="4.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="8" max="10" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="12" max="12" style="1" width="10.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="4.7109375" collapsed="true"/>
+    <col min="17" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -725,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -763,10 +799,10 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -775,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -810,7 +846,10 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>92</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -819,7 +858,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>17</v>
@@ -854,7 +893,10 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>93</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
@@ -895,7 +937,10 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -936,6 +981,9 @@
         <v>73</v>
       </c>
       <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -945,7 +993,7 @@
         <v>71</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>20</v>
@@ -980,7 +1028,10 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>96</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
@@ -989,7 +1040,7 @@
         <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>22</v>
@@ -1024,7 +1075,10 @@
         <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>97</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
@@ -1033,7 +1087,7 @@
         <v>72</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>24</v>
@@ -1068,7 +1122,10 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>98</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>5</v>
@@ -1077,7 +1134,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>25</v>
@@ -1112,7 +1169,10 @@
         <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>99</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
@@ -1121,7 +1181,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>26</v>
@@ -1156,7 +1216,10 @@
         <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
@@ -1165,7 +1228,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>27</v>
@@ -1200,7 +1263,10 @@
         <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>5</v>
@@ -1209,7 +1275,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>28</v>
@@ -1242,7 +1308,7 @@
   </sheetData>
   <autoFilter ref="E1:E12" xr:uid="{33F8F8F8-AE16-4B12-9448-CA2FBF5C7D40}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>